<commit_message>
to object oriented 2.2 seperate excel files full text
</commit_message>
<xml_diff>
--- a/companies_glossary/HUL.xlsx
+++ b/companies_glossary/HUL.xlsx
@@ -370,32 +370,50 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>8</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>frequency</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>lemma</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>pos</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>eng-tag</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>dependency</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>afinn sentiment</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>mcdonals sentiment</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>token id</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -3594,32 +3612,50 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>8</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>frequency</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>lemma</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>pos</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>eng-tag</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>dependency</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>afinn sentiment</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>mcdonals sentiment</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>token id</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -5004,32 +5040,50 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>8</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>frequency</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>lemma</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>pos</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>eng-tag</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>dependency</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>afinn sentiment</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>mcdonals sentiment</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>token id</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -5364,32 +5418,50 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>8</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>frequency</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>lemma</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>pos</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>eng-tag</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>dependency</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>afinn sentiment</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>mcdonals sentiment</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>token id</t>
+        </is>
       </c>
     </row>
     <row r="2">

</xml_diff>